<commit_message>
Planif finie, Rapport A5 fini ?, letzgo
</commit_message>
<xml_diff>
--- a/Projet/PlannificationPrevisionnelle.xlsx
+++ b/Projet/PlannificationPrevisionnelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Perso\Bureau\Travail\BUT-Info\S2\S2-05-Gestion_d_un_projet\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40123DA5-B138-4605-9118-255C311F28DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E37AD36-B5DE-42C4-B1B3-737D0F5E0048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>Choses à faire</t>
   </si>
@@ -51,21 +51,12 @@
     <t>Problèmes rencontrés</t>
   </si>
   <si>
-    <t>Date début prévue</t>
-  </si>
-  <si>
-    <t>Date fin prévue</t>
-  </si>
-  <si>
     <t>Date fin effective</t>
   </si>
   <si>
     <t>Bilan</t>
   </si>
   <si>
-    <t>Date début effective</t>
-  </si>
-  <si>
     <t>Date du rendu final : 13/06/2022</t>
   </si>
   <si>
@@ -87,15 +78,6 @@
     <t>Recherche trop globale</t>
   </si>
   <si>
-    <t>Très tardif et fait de manière peu homogène</t>
-  </si>
-  <si>
-    <t>Maquette de base bancale + collaboration difficile</t>
-  </si>
-  <si>
-    <t>Trop de détails (n'est pas une décomposition fonctionnelle)</t>
-  </si>
-  <si>
     <t>1. Analyse</t>
   </si>
   <si>
@@ -108,9 +90,6 @@
     <t>1.6 Étude des coûts</t>
   </si>
   <si>
-    <t>1.2. Veille technologique des technologies à utiliser</t>
-  </si>
-  <si>
     <t>2. Conception</t>
   </si>
   <si>
@@ -226,13 +205,62 @@
   </si>
   <si>
     <t>3.4.2 Finalisation</t>
+  </si>
+  <si>
+    <t>Guillaume</t>
+  </si>
+  <si>
+    <t>Guillaume, Alexandre</t>
+  </si>
+  <si>
+    <t>Kepa, Nicolas</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Début S4</t>
+  </si>
+  <si>
+    <t>Milieu S4</t>
+  </si>
+  <si>
+    <t>Fin S4</t>
+  </si>
+  <si>
+    <t>1.2. Veille technologique des
+technologies à utiliser</t>
+  </si>
+  <si>
+    <t>Trop de détails (n'est pas une 
+décomposition fonctionnelle)</t>
+  </si>
+  <si>
+    <t>Très tardif et fait de manière 
+peu homogène</t>
+  </si>
+  <si>
+    <t>Maquette de base bancale 
++ collaboration difficile</t>
+  </si>
+  <si>
+    <t>Date début
+prévue</t>
+  </si>
+  <si>
+    <t>Date début
+effective</t>
+  </si>
+  <si>
+    <t>Date fin
+prévue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,12 +278,6 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -341,16 +363,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -359,14 +377,10 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -381,17 +395,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -677,18 +715,17 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:H9"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" customWidth="1"/>
     <col min="8" max="8" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="43.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
@@ -700,211 +737,211 @@
     <col min="19" max="19" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4">
+        <v>44602</v>
+      </c>
+      <c r="E3" s="4">
+        <v>44602</v>
+      </c>
+      <c r="F3" s="4">
+        <v>44607</v>
+      </c>
+      <c r="G3" s="3">
+        <v>44604</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="4">
+        <v>44602</v>
+      </c>
+      <c r="E4" s="4">
+        <v>44602</v>
+      </c>
+      <c r="F4" s="4">
+        <v>44607</v>
+      </c>
+      <c r="G4" s="4">
+        <v>44604</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="4">
+        <v>44632</v>
+      </c>
+      <c r="E5" s="4">
+        <v>44632</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44640</v>
+      </c>
+      <c r="G5" s="3">
+        <v>44676</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44638</v>
+      </c>
+      <c r="E6" s="3">
+        <v>44638</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44661</v>
+      </c>
+      <c r="G6" s="3">
+        <v>44682</v>
+      </c>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="3">
+        <v>44661</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44632</v>
+      </c>
+      <c r="F7" s="3">
+        <v>44681</v>
+      </c>
+      <c r="G7" s="3">
+        <v>44680</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="4">
+        <v>44701</v>
+      </c>
+      <c r="E8" s="4">
+        <v>44718</v>
+      </c>
+      <c r="F8" s="4">
+        <v>44706</v>
+      </c>
+      <c r="G8" s="4">
+        <v>44719</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="6">
-        <v>44602</v>
-      </c>
-      <c r="E3" s="6">
-        <v>44602</v>
-      </c>
-      <c r="F3" s="6">
-        <v>44607</v>
-      </c>
-      <c r="G3" s="5">
-        <v>44604</v>
-      </c>
-      <c r="H3" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="6">
-        <v>44602</v>
-      </c>
-      <c r="E4" s="6">
-        <v>44602</v>
-      </c>
-      <c r="F4" s="6">
-        <v>44607</v>
-      </c>
-      <c r="G4" s="6">
-        <v>44604</v>
-      </c>
-      <c r="H4" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6">
-        <v>44632</v>
-      </c>
-      <c r="E5" s="6">
-        <v>44632</v>
-      </c>
-      <c r="F5" s="5">
-        <v>44640</v>
-      </c>
-      <c r="G5" s="5">
-        <v>44676</v>
-      </c>
-      <c r="H5" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="5">
-        <v>44638</v>
-      </c>
-      <c r="E6" s="5">
-        <v>44638</v>
-      </c>
-      <c r="F6" s="5">
-        <v>44661</v>
-      </c>
-      <c r="G6" s="5">
-        <v>44682</v>
-      </c>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="7" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5">
-        <v>44661</v>
-      </c>
-      <c r="E7" s="5">
-        <v>44632</v>
-      </c>
-      <c r="F7" s="5">
-        <v>44681</v>
-      </c>
-      <c r="G7" s="5">
-        <v>44680</v>
-      </c>
-      <c r="H7" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="6">
-        <v>44701</v>
-      </c>
-      <c r="E8" s="6">
-        <v>44718</v>
-      </c>
-      <c r="F8" s="6">
-        <v>44706</v>
-      </c>
-      <c r="G8" s="6">
-        <v>44719</v>
-      </c>
-      <c r="H8" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="18">
+      <c r="H9" s="12">
         <f>AVERAGE(H3:H8)</f>
         <v>1</v>
       </c>
@@ -923,124 +960,123 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C1B143-4A5A-4F4F-860C-E793F1A07474}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="A2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="3">
+        <v>54</v>
+      </c>
+      <c r="H3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="3">
+        <v>54</v>
+      </c>
+      <c r="H4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="3">
+        <v>54</v>
+      </c>
+      <c r="H5" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="18">
+      <c r="H6" s="12">
         <f>AVERAGE(H3:H5)</f>
         <v>0</v>
       </c>
@@ -1050,7 +1086,7 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A6:F6"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1060,233 +1096,440 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="A2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="A16" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="12">
+        <f>SUM(H3:H5,H9,H24,H25,H26,H28,H27,H24,H25)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" ht="16.8" x14ac:dyDescent="0.4"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A29:F29"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>